<commit_message>
Updated to fetch data from excel using DataProvider
</commit_message>
<xml_diff>
--- a/freeCRM/src/main/java/TestData/Deals.xlsx
+++ b/freeCRM/src/main/java/TestData/Deals.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Deals" sheetId="1" r:id="rId1"/>
-    <sheet name="login_with_invalid_data" sheetId="2" r:id="rId2"/>
+    <sheet name="new_deal" sheetId="1" r:id="rId1"/>
+    <sheet name="edit_deal" sheetId="3" r:id="rId2"/>
+    <sheet name="login_with_invalid_data" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t>username</t>
   </si>
@@ -63,6 +64,12 @@
   </si>
   <si>
     <t>Updated deal</t>
+  </si>
+  <si>
+    <t>Exclude Reports?</t>
+  </si>
+  <si>
+    <t>true</t>
   </si>
 </sst>
 </file>
@@ -119,10 +126,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -425,88 +435,137 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:H2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" customWidth="1"/>
-    <col min="6" max="6" width="13.5703125" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" style="4" customWidth="1"/>
+    <col min="2" max="5" width="9.140625" style="4"/>
+    <col min="6" max="6" width="19.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="18.28515625" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6">
+      <c r="A1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-    </row>
-    <row r="2" spans="1:17">
-      <c r="A2" s="1" t="s">
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B2" s="1">
+      <c r="B2" s="5">
         <v>2000</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2" s="5">
         <v>2</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
-      <c r="J2" s="1"/>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-      <c r="M2" s="1"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
-      <c r="Q2" s="1"/>
+      <c r="F2" s="5" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" style="4" customWidth="1"/>
+    <col min="2" max="5" width="9.140625" style="4"/>
+    <col min="6" max="6" width="19.140625" style="4" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="4"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="5">
+        <v>2000</v>
+      </c>
+      <c r="C2" s="5">
+        <v>2</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="5" t="b">
+        <v>1</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B4"/>
   <sheetViews>

</xml_diff>